<commit_message>
Pandas: Análise de ROI
</commit_message>
<xml_diff>
--- a/pandas/marketing/marketing.xlsx
+++ b/pandas/marketing/marketing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\python_intro\pandas\marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340622B9-BF74-4C91-ADD4-1D047831FBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C197972-0AAC-459C-9307-7442C61D7C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{4F107EC4-5A8D-4CF3-86EA-B2B573C5AE26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4F107EC4-5A8D-4CF3-86EA-B2B573C5AE26}"/>
   </bookViews>
   <sheets>
     <sheet name="clientes" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>custo</t>
   </si>
   <si>
-    <t>rececita</t>
-  </si>
-  <si>
     <t>data_lancamento</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>Campanha Especial</t>
+  </si>
+  <si>
+    <t>receita</t>
   </si>
 </sst>
 </file>
@@ -280,6 +280,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -385,22 +388,28 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -491,15 +500,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -518,35 +518,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7138FF4-EA16-4733-A1AA-48A64B682E9B}" name="Tabela1" displayName="Tabela1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="24" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7138FF4-EA16-4733-A1AA-48A64B682E9B}" name="Tabela1" displayName="Tabela1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:E11" xr:uid="{E7138FF4-EA16-4733-A1AA-48A64B682E9B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9C3EF12A-308F-4277-A537-B9B744ACF79E}" name="id _cliente" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{354FD4A0-34CC-48A9-812B-06AA63F206AF}" name="nome " dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{7542BB76-E73D-40EF-A7D6-108673297C21}" name="idade " dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{FAC193D4-A9BF-4A3D-AB56-4D68E765E237}" name="localização" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{96861E7C-2066-4448-BFD4-22248B5969F7}" name="data_cadastro" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{9C3EF12A-308F-4277-A537-B9B744ACF79E}" name="id _cliente" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{354FD4A0-34CC-48A9-812B-06AA63F206AF}" name="nome " dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{7542BB76-E73D-40EF-A7D6-108673297C21}" name="idade " dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{FAC193D4-A9BF-4A3D-AB56-4D68E765E237}" name="localização" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{96861E7C-2066-4448-BFD4-22248B5969F7}" name="data_cadastro" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F7D02C43-AF26-42DF-9066-E2360C45E552}" name="Tabela2" displayName="Tabela2" ref="A1:E9" totalsRowShown="0" headerRowDxfId="27" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F7D02C43-AF26-42DF-9066-E2360C45E552}" name="Tabela2" displayName="Tabela2" ref="A1:E9" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:E9" xr:uid="{F7D02C43-AF26-42DF-9066-E2360C45E552}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F0B6D5BC-6E94-4290-A4F0-3BB08E1E1ACD}" name="id_campanha" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{82ABB198-F5CD-47E1-8FB6-87FDD23AB446}" name="nome_campanha" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{7DA8A32A-2134-4E80-939E-D22C8581E0AC}" name="custo" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{F74265BD-16E1-49E9-BD5E-45161D29EA9A}" name="rececita" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{38D07255-2B6D-47C4-A4AD-2334C239BF79}" name="data_lancamento" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{F0B6D5BC-6E94-4290-A4F0-3BB08E1E1ACD}" name="id_campanha" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{82ABB198-F5CD-47E1-8FB6-87FDD23AB446}" name="nome_campanha" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{7DA8A32A-2134-4E80-939E-D22C8581E0AC}" name="custo" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{F74265BD-16E1-49E9-BD5E-45161D29EA9A}" name="receita" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{38D07255-2B6D-47C4-A4AD-2334C239BF79}" name="data_lancamento" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4A5B4FF6-F959-4671-8D8D-C8F5DE4ABAEF}" name="Tabela3" displayName="Tabela3" ref="A1:F16" totalsRowShown="0" headerRowDxfId="26" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4A5B4FF6-F959-4671-8D8D-C8F5DE4ABAEF}" name="Tabela3" displayName="Tabela3" ref="A1:F16" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:F16" xr:uid="{4A5B4FF6-F959-4671-8D8D-C8F5DE4ABAEF}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B982FEE2-C281-4A5A-99D4-D781000B4FC6}" name="id_vendas" dataDxfId="11"/>
@@ -561,13 +561,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A49C00D-D7D5-445B-8305-9DDE0710F37C}" name="Tabela4" displayName="Tabela4" ref="A1:D8" totalsRowShown="0" headerRowDxfId="25" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A49C00D-D7D5-445B-8305-9DDE0710F37C}" name="Tabela4" displayName="Tabela4" ref="A1:D8" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D8" xr:uid="{4A49C00D-D7D5-445B-8305-9DDE0710F37C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DC1CD740-0C31-4EDD-BEEC-47A1FF618ABD}" name="id_produto" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{CAEE7D15-172C-4740-9527-987405F03D7E}" name="nome_produto" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{6D8726AD-CF70-4268-9307-976CD26898C4}" name="categoria" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{41F3EDA9-EB54-4E2B-BF7A-9F9B9FB39EEE}" name="preco" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{DC1CD740-0C31-4EDD-BEEC-47A1FF618ABD}" name="id_produto" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{CAEE7D15-172C-4740-9527-987405F03D7E}" name="nome_produto" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{6D8726AD-CF70-4268-9307-976CD26898C4}" name="categoria" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{41F3EDA9-EB54-4E2B-BF7A-9F9B9FB39EEE}" name="preco" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -977,13 +977,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="4">
         <v>50</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="5">
         <v>43999</v>
@@ -994,13 +994,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4">
         <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="5">
         <v>45041</v>
@@ -1011,13 +1011,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="4">
         <v>38</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="5">
         <v>44867</v>
@@ -1028,13 +1028,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="4">
         <v>31</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="5">
         <v>44539</v>
@@ -1045,13 +1045,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="4">
         <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="5">
         <v>44635</v>
@@ -1062,13 +1062,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="4">
         <v>22</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="5">
         <v>44931</v>
@@ -1079,13 +1079,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4">
         <v>33</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="5">
         <v>44790</v>
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18865D6-BA79-45CE-865B-685368F696A4}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,10 +1127,10 @@
         <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1138,7 +1138,7 @@
         <v>101</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1">
         <v>10000</v>
@@ -1155,7 +1155,7 @@
         <v>102</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1">
         <v>15000</v>
@@ -1172,7 +1172,7 @@
         <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1">
         <v>20000</v>
@@ -1189,7 +1189,7 @@
         <v>104</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1">
         <v>12000</v>
@@ -1206,7 +1206,7 @@
         <v>105</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="1">
         <v>9000</v>
@@ -1223,7 +1223,7 @@
         <v>106</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1">
         <v>8000</v>
@@ -1240,7 +1240,7 @@
         <v>107</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1">
         <v>7000</v>
@@ -1257,7 +1257,7 @@
         <v>108</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1">
         <v>18000</v>
@@ -1297,22 +1297,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1392,7 +1392,7 @@
         <v>101</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1412,7 +1412,7 @@
         <v>102</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
         <v>103</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1452,7 +1452,7 @@
         <v>101</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
         <v>102</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1492,7 +1492,7 @@
         <v>103</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1512,7 +1512,7 @@
         <v>101</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1572,7 +1572,7 @@
         <v>101</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1592,7 +1592,7 @@
         <v>102</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1612,7 +1612,7 @@
         <v>103</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1627,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA05627C-4333-42DA-B34D-9DD5D5B2C2C9}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,16 +1642,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1659,10 +1659,10 @@
         <v>101</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D2" s="1">
         <v>300</v>
@@ -1673,10 +1673,10 @@
         <v>102</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D3" s="1">
         <v>450</v>
@@ -1687,10 +1687,10 @@
         <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1">
         <v>200</v>
@@ -1701,10 +1701,10 @@
         <v>104</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1">
         <v>600</v>
@@ -1715,10 +1715,10 @@
         <v>105</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1">
         <v>500</v>
@@ -1729,10 +1729,10 @@
         <v>106</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1">
         <v>350</v>
@@ -1743,10 +1743,10 @@
         <v>107</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1">
         <v>800</v>

</xml_diff>

<commit_message>
Pandas: alimentando planilha de dados e gerando relatório de produtos mais vendidos
</commit_message>
<xml_diff>
--- a/pandas/marketing/marketing.xlsx
+++ b/pandas/marketing/marketing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\python_intro\pandas\marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C197972-0AAC-459C-9307-7442C61D7C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6858470-1E04-423A-A09F-4B057CEC056F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4F107EC4-5A8D-4CF3-86EA-B2B573C5AE26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{4F107EC4-5A8D-4CF3-86EA-B2B573C5AE26}"/>
   </bookViews>
   <sheets>
     <sheet name="clientes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="86">
   <si>
     <t>id _cliente</t>
   </si>
@@ -207,14 +207,112 @@
   </si>
   <si>
     <t>receita</t>
+  </si>
+  <si>
+    <t>Juliana Pereira</t>
+  </si>
+  <si>
+    <t>Marcos Oliveira</t>
+  </si>
+  <si>
+    <t>Renata Costa</t>
+  </si>
+  <si>
+    <t>Gustavo Rocha</t>
+  </si>
+  <si>
+    <t>Clara Martins</t>
+  </si>
+  <si>
+    <t>Leandro Santos</t>
+  </si>
+  <si>
+    <t>Mariana Oliveira</t>
+  </si>
+  <si>
+    <t>Felipe Alves</t>
+  </si>
+  <si>
+    <t>Simone Lima</t>
+  </si>
+  <si>
+    <t>Igor Fernandes</t>
+  </si>
+  <si>
+    <t>Dia das Mães 2023</t>
+  </si>
+  <si>
+    <t>Carnaval 2023</t>
+  </si>
+  <si>
+    <t>Black Friday 2021</t>
+  </si>
+  <si>
+    <t>Natal 2022</t>
+  </si>
+  <si>
+    <t>Dia dos Namorados 2023</t>
+  </si>
+  <si>
+    <t>Black Friday 2020</t>
+  </si>
+  <si>
+    <t>Super Ofertas 2023</t>
+  </si>
+  <si>
+    <t>Halloween 2023</t>
+  </si>
+  <si>
+    <t>Super Promoção 2023</t>
+  </si>
+  <si>
+    <t>Dia das Crianças 2023</t>
+  </si>
+  <si>
+    <t>Planejamento Estratégico</t>
+  </si>
+  <si>
+    <t>Anúncio Básico</t>
+  </si>
+  <si>
+    <t>Consultoria Avançada</t>
+  </si>
+  <si>
+    <t>Design de Marca</t>
+  </si>
+  <si>
+    <t>Publicidade Digital</t>
+  </si>
+  <si>
+    <t>Gestão de Mídias</t>
+  </si>
+  <si>
+    <t>Publicidade Premium</t>
+  </si>
+  <si>
+    <t>Branding Digital</t>
+  </si>
+  <si>
+    <t>Anúncio Social</t>
+  </si>
+  <si>
+    <t>Consultoria VIP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -242,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -259,6 +357,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,8 +619,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7138FF4-EA16-4733-A1AA-48A64B682E9B}" name="Tabela1" displayName="Tabela1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:E11" xr:uid="{E7138FF4-EA16-4733-A1AA-48A64B682E9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7138FF4-EA16-4733-A1AA-48A64B682E9B}" name="Tabela1" displayName="Tabela1" ref="A1:E21" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:E21" xr:uid="{E7138FF4-EA16-4733-A1AA-48A64B682E9B}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9C3EF12A-308F-4277-A537-B9B744ACF79E}" name="id _cliente" dataDxfId="25"/>
     <tableColumn id="2" xr3:uid="{354FD4A0-34CC-48A9-812B-06AA63F206AF}" name="nome " dataDxfId="24"/>
@@ -532,8 +633,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F7D02C43-AF26-42DF-9066-E2360C45E552}" name="Tabela2" displayName="Tabela2" ref="A1:E9" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:E9" xr:uid="{F7D02C43-AF26-42DF-9066-E2360C45E552}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F7D02C43-AF26-42DF-9066-E2360C45E552}" name="Tabela2" displayName="Tabela2" ref="A1:E19" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:E19" xr:uid="{F7D02C43-AF26-42DF-9066-E2360C45E552}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{F0B6D5BC-6E94-4290-A4F0-3BB08E1E1ACD}" name="id_campanha" dataDxfId="18"/>
     <tableColumn id="2" xr3:uid="{82ABB198-F5CD-47E1-8FB6-87FDD23AB446}" name="nome_campanha" dataDxfId="17"/>
@@ -546,8 +647,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4A5B4FF6-F959-4671-8D8D-C8F5DE4ABAEF}" name="Tabela3" displayName="Tabela3" ref="A1:F16" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:F16" xr:uid="{4A5B4FF6-F959-4671-8D8D-C8F5DE4ABAEF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4A5B4FF6-F959-4671-8D8D-C8F5DE4ABAEF}" name="Tabela3" displayName="Tabela3" ref="A1:F31" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:F31" xr:uid="{4A5B4FF6-F959-4671-8D8D-C8F5DE4ABAEF}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B982FEE2-C281-4A5A-99D4-D781000B4FC6}" name="id_vendas" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{5ED6A4D0-9A26-46E7-9180-D395D1A21A19}" name="id_cliente" dataDxfId="10"/>
@@ -561,8 +662,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A49C00D-D7D5-445B-8305-9DDE0710F37C}" name="Tabela4" displayName="Tabela4" ref="A1:D8" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D8" xr:uid="{4A49C00D-D7D5-445B-8305-9DDE0710F37C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A49C00D-D7D5-445B-8305-9DDE0710F37C}" name="Tabela4" displayName="Tabela4" ref="A1:D18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D18" xr:uid="{4A49C00D-D7D5-445B-8305-9DDE0710F37C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{DC1CD740-0C31-4EDD-BEEC-47A1FF618ABD}" name="id_produto" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{CAEE7D15-172C-4740-9527-987405F03D7E}" name="nome_produto" dataDxfId="2"/>
@@ -890,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE1CC0B-D520-4A30-BF2F-4B45C7FB6949}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,20 +1192,191 @@
         <v>44790</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="4">
+        <v>28</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="5">
+        <v>45067</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="6">
+        <v>39</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="5">
+        <v>44380</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="4">
+        <v>25</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="5">
+        <v>45210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="4">
+        <v>42</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="5">
+        <v>44609</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="4">
+        <v>29</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="5">
+        <v>44940</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="4">
+        <v>35</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="5">
+        <v>44812</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="4">
+        <v>30</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="5">
+        <v>45015</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="4">
+        <v>46</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="5">
+        <v>44734</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="4">
+        <v>24</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="5">
+        <v>44517</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="4">
+        <v>37</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="5">
+        <v>44686</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18865D6-BA79-45CE-865B-685368F696A4}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,6 +1541,176 @@
         <v>45245</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>109</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12000</v>
+      </c>
+      <c r="D10" s="1">
+        <v>40000</v>
+      </c>
+      <c r="E10" s="3">
+        <v>45054</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>110</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="1">
+        <v>15000</v>
+      </c>
+      <c r="D11" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E11" s="3">
+        <v>44972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>111</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="1">
+        <v>18000</v>
+      </c>
+      <c r="D12" s="1">
+        <v>65000</v>
+      </c>
+      <c r="E12" s="3">
+        <v>44526</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>112</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="1">
+        <v>22000</v>
+      </c>
+      <c r="D13" s="1">
+        <v>55000</v>
+      </c>
+      <c r="E13" s="3">
+        <v>44905</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>113</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="1">
+        <v>7000</v>
+      </c>
+      <c r="D14" s="1">
+        <v>25000</v>
+      </c>
+      <c r="E14" s="3">
+        <v>45089</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>114</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="1">
+        <v>17000</v>
+      </c>
+      <c r="D15" s="1">
+        <v>60000</v>
+      </c>
+      <c r="E15" s="3">
+        <v>44162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>115</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="1">
+        <v>13000</v>
+      </c>
+      <c r="D16" s="1">
+        <v>45000</v>
+      </c>
+      <c r="E16" s="3">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>116</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="1">
+        <v>9000</v>
+      </c>
+      <c r="D17" s="1">
+        <v>30000</v>
+      </c>
+      <c r="E17" s="3">
+        <v>45230</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>117</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="1">
+        <v>11000</v>
+      </c>
+      <c r="D18" s="1">
+        <v>35000</v>
+      </c>
+      <c r="E18" s="3">
+        <v>45170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>118</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="1">
+        <v>8000</v>
+      </c>
+      <c r="D19" s="1">
+        <v>25000</v>
+      </c>
+      <c r="E19" s="3">
+        <v>45211</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
@@ -1279,10 +1721,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1601F194-A0E2-4FDF-AD8F-A1A11A03170A}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,6 +2057,306 @@
         <v>35</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>7</v>
+      </c>
+      <c r="C17" s="4">
+        <v>350</v>
+      </c>
+      <c r="D17" s="5">
+        <v>45240</v>
+      </c>
+      <c r="E17" s="4">
+        <v>101</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4">
+        <v>8</v>
+      </c>
+      <c r="C18" s="4">
+        <v>200</v>
+      </c>
+      <c r="D18" s="5">
+        <v>45245</v>
+      </c>
+      <c r="E18" s="4">
+        <v>102</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <v>9</v>
+      </c>
+      <c r="C19" s="4">
+        <v>450</v>
+      </c>
+      <c r="D19" s="5">
+        <v>45265</v>
+      </c>
+      <c r="E19" s="4">
+        <v>110</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4">
+        <v>10</v>
+      </c>
+      <c r="C20" s="4">
+        <v>500</v>
+      </c>
+      <c r="D20" s="5">
+        <v>45278</v>
+      </c>
+      <c r="E20" s="4">
+        <v>101</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4">
+        <v>600</v>
+      </c>
+      <c r="D21" s="5">
+        <v>45293</v>
+      </c>
+      <c r="E21" s="4">
+        <v>105</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4">
+        <v>250</v>
+      </c>
+      <c r="D22" s="5">
+        <v>45299</v>
+      </c>
+      <c r="E22" s="4">
+        <v>103</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4">
+        <v>3</v>
+      </c>
+      <c r="C23" s="4">
+        <v>400</v>
+      </c>
+      <c r="D23" s="5">
+        <v>45311</v>
+      </c>
+      <c r="E23" s="4">
+        <v>110</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4">
+        <v>4</v>
+      </c>
+      <c r="C24" s="4">
+        <v>550</v>
+      </c>
+      <c r="D24" s="5">
+        <v>45316</v>
+      </c>
+      <c r="E24" s="4">
+        <v>102</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4">
+        <v>5</v>
+      </c>
+      <c r="C25" s="4">
+        <v>700</v>
+      </c>
+      <c r="D25" s="5">
+        <v>45332</v>
+      </c>
+      <c r="E25" s="4">
+        <v>105</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4">
+        <v>6</v>
+      </c>
+      <c r="C26" s="4">
+        <v>300</v>
+      </c>
+      <c r="D26" s="5">
+        <v>45340</v>
+      </c>
+      <c r="E26" s="4">
+        <v>107</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4">
+        <v>7</v>
+      </c>
+      <c r="C27" s="4">
+        <v>450</v>
+      </c>
+      <c r="D27" s="5">
+        <v>45350</v>
+      </c>
+      <c r="E27" s="4">
+        <v>106</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4">
+        <v>8</v>
+      </c>
+      <c r="C28" s="4">
+        <v>500</v>
+      </c>
+      <c r="D28" s="5">
+        <v>45356</v>
+      </c>
+      <c r="E28" s="4">
+        <v>103</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4">
+        <v>9</v>
+      </c>
+      <c r="C29" s="4">
+        <v>350</v>
+      </c>
+      <c r="D29" s="5">
+        <v>45361</v>
+      </c>
+      <c r="E29" s="4">
+        <v>101</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4">
+        <v>10</v>
+      </c>
+      <c r="C30" s="4">
+        <v>600</v>
+      </c>
+      <c r="D30" s="5">
+        <v>45366</v>
+      </c>
+      <c r="E30" s="4">
+        <v>102</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4">
+        <v>700</v>
+      </c>
+      <c r="D31" s="5">
+        <v>45376</v>
+      </c>
+      <c r="E31" s="4">
+        <v>103</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
@@ -1625,10 +2367,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA05627C-4333-42DA-B34D-9DD5D5B2C2C9}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,7 +2473,7 @@
       <c r="B7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="1">
@@ -1750,6 +2492,146 @@
       </c>
       <c r="D8" s="1">
         <v>800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>108</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>109</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>110</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>111</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>112</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>113</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>114</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>115</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>116</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>117</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>